<commit_message>
Fix warnings on pre production
</commit_message>
<xml_diff>
--- a/Back-End-Flask/Hiru_flask/Durability-predictionDatset.xlsx
+++ b/Back-End-Flask/Hiru_flask/Durability-predictionDatset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research_2024\Code_base\Final Project\Final_project_056\Back-End-Flask\Hiru_flask\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D123C3-C882-44FA-9F0E-1F094B8519D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17473C10-529E-479F-8F6A-8C0CBA9970A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1662,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A861" workbookViewId="0">
+      <selection activeCell="C897" sqref="C897"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1696,7 +1696,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>22.171794871794901</v>
+        <v>30.171794871794901</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -1716,7 +1716,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>22.141025641025639</v>
+        <v>33.1410256410256</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -1736,7 +1736,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>22.171794871794869</v>
+        <v>23.171794871794901</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -1756,7 +1756,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>22.110256410256412</v>
+        <v>24.110256410256401</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -1776,7 +1776,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>22.125641025641031</v>
+        <v>25.125641025640999</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -1796,7 +1796,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>22.187179487179488</v>
+        <v>34.187179487179499</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -1816,7 +1816,7 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>22.171794871794869</v>
+        <v>22.171794871794901</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -1836,7 +1836,7 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>22.141025641025639</v>
+        <v>20.1410256410256</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -1876,7 +1876,7 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>22.110256410256412</v>
+        <v>28.110256410256401</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -1916,7 +1916,7 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>22.187179487179488</v>
+        <v>29.187179487179499</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -1936,7 +1936,7 @@
         <v>4</v>
       </c>
       <c r="C14">
-        <v>22.171794871794869</v>
+        <v>21.171794871794901</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1976,7 +1976,7 @@
         <v>6</v>
       </c>
       <c r="C16">
-        <v>22.171794871794869</v>
+        <v>20.171794871794901</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -1996,7 +1996,7 @@
         <v>7</v>
       </c>
       <c r="C17">
-        <v>22.110256410256412</v>
+        <v>29.110256410256401</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
@@ -2036,7 +2036,7 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>22.187179487179488</v>
+        <v>30.187179487179499</v>
       </c>
       <c r="D19" t="s">
         <v>16</v>
@@ -2056,7 +2056,7 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <v>22.171794871794869</v>
+        <v>23.171794871794901</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
@@ -2076,7 +2076,7 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <v>22.141025641025639</v>
+        <v>24.1410256410256</v>
       </c>
       <c r="D21" t="s">
         <v>16</v>
@@ -2116,7 +2116,7 @@
         <v>7</v>
       </c>
       <c r="C23">
-        <v>22.110256410256412</v>
+        <v>27.110256410256401</v>
       </c>
       <c r="D23" t="s">
         <v>16</v>
@@ -2156,7 +2156,7 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>22.187179487179488</v>
+        <v>23.187179487179499</v>
       </c>
       <c r="D25" t="s">
         <v>16</v>
@@ -2176,7 +2176,7 @@
         <v>4</v>
       </c>
       <c r="C26">
-        <v>22.171794871794869</v>
+        <v>24.171794871794901</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
@@ -2236,7 +2236,7 @@
         <v>7</v>
       </c>
       <c r="C29">
-        <v>22.110256410256412</v>
+        <v>26.110256410256401</v>
       </c>
       <c r="D29" t="s">
         <v>16</v>
@@ -2276,7 +2276,7 @@
         <v>9</v>
       </c>
       <c r="C31">
-        <v>22.187179487179488</v>
+        <v>17.187179487179499</v>
       </c>
       <c r="D31" t="s">
         <v>16</v>
@@ -2536,7 +2536,7 @@
         <v>21</v>
       </c>
       <c r="C44">
-        <v>22.76923076923077</v>
+        <v>29.769230769230798</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
@@ -2616,7 +2616,7 @@
         <v>25</v>
       </c>
       <c r="C48">
-        <v>22.76923076923077</v>
+        <v>27.769230769230798</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
@@ -2756,7 +2756,7 @@
         <v>25</v>
       </c>
       <c r="C55">
-        <v>22.76923076923077</v>
+        <v>26.769230769230798</v>
       </c>
       <c r="D55" t="s">
         <v>16</v>
@@ -2816,7 +2816,7 @@
         <v>21</v>
       </c>
       <c r="C58">
-        <v>22.76923076923077</v>
+        <v>28.769230769230798</v>
       </c>
       <c r="D58" t="s">
         <v>16</v>
@@ -3596,7 +3596,7 @@
         <v>7</v>
       </c>
       <c r="C97">
-        <v>14.533333333333321</v>
+        <v>14.533333333333299</v>
       </c>
       <c r="D97" t="s">
         <v>16</v>
@@ -5356,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="C185">
-        <v>14.48717948717948</v>
+        <v>13.4871794871795</v>
       </c>
       <c r="D185" t="s">
         <v>16</v>
@@ -5596,7 +5596,7 @@
         <v>5</v>
       </c>
       <c r="C197">
-        <v>14.48717948717948</v>
+        <v>13.4871794871795</v>
       </c>
       <c r="D197" t="s">
         <v>16</v>
@@ -5796,7 +5796,7 @@
         <v>5</v>
       </c>
       <c r="C207">
-        <v>14.61538461538461</v>
+        <v>18.615384615384599</v>
       </c>
       <c r="D207" t="s">
         <v>62</v>
@@ -6216,7 +6216,7 @@
         <v>5</v>
       </c>
       <c r="C228">
-        <v>14.61538461538461</v>
+        <v>15.615384615384601</v>
       </c>
       <c r="D228" t="s">
         <v>410</v>
@@ -6996,7 +6996,7 @@
         <v>4</v>
       </c>
       <c r="C267">
-        <v>22.158974358974358</v>
+        <v>18.158974358974401</v>
       </c>
       <c r="D267" t="s">
         <v>16</v>
@@ -7056,7 +7056,7 @@
         <v>7</v>
       </c>
       <c r="C270">
-        <v>22.097435897435901</v>
+        <v>23.097435897435901</v>
       </c>
       <c r="D270" t="s">
         <v>16</v>
@@ -7076,7 +7076,7 @@
         <v>8</v>
       </c>
       <c r="C271">
-        <v>22.112820512820509</v>
+        <v>20.112820512820502</v>
       </c>
       <c r="D271" t="s">
         <v>16</v>
@@ -7096,7 +7096,7 @@
         <v>9</v>
       </c>
       <c r="C272">
-        <v>22.17435897435897</v>
+        <v>21.174358974358999</v>
       </c>
       <c r="D272" t="s">
         <v>16</v>
@@ -7116,7 +7116,7 @@
         <v>4</v>
       </c>
       <c r="C273">
-        <v>22.158974358974358</v>
+        <v>21.158974358974401</v>
       </c>
       <c r="D273" t="s">
         <v>16</v>
@@ -7136,7 +7136,7 @@
         <v>73</v>
       </c>
       <c r="C274">
-        <v>22.14358974358974</v>
+        <v>21.1435897435897</v>
       </c>
       <c r="D274" t="s">
         <v>16</v>
@@ -7176,7 +7176,7 @@
         <v>7</v>
       </c>
       <c r="C276">
-        <v>22.097435897435901</v>
+        <v>23.097435897435901</v>
       </c>
       <c r="D276" t="s">
         <v>16</v>
@@ -7196,7 +7196,7 @@
         <v>8</v>
       </c>
       <c r="C277">
-        <v>22.112820512820509</v>
+        <v>25.112820512820502</v>
       </c>
       <c r="D277" t="s">
         <v>16</v>
@@ -7216,7 +7216,7 @@
         <v>9</v>
       </c>
       <c r="C278">
-        <v>22.17435897435897</v>
+        <v>26.174358974358999</v>
       </c>
       <c r="D278" t="s">
         <v>16</v>
@@ -7236,7 +7236,7 @@
         <v>4</v>
       </c>
       <c r="C279">
-        <v>22.158974358974358</v>
+        <v>25.158974358974401</v>
       </c>
       <c r="D279" t="s">
         <v>16</v>
@@ -7356,7 +7356,7 @@
         <v>4</v>
       </c>
       <c r="C285">
-        <v>22.158974358974358</v>
+        <v>21.158974358974401</v>
       </c>
       <c r="D285" t="s">
         <v>17</v>
@@ -19656,7 +19656,7 @@
         <v>172</v>
       </c>
       <c r="C900">
-        <v>23.769230769230759</v>
+        <v>28.769230769230798</v>
       </c>
       <c r="D900" t="s">
         <v>16</v>
@@ -21496,7 +21496,7 @@
         <v>235</v>
       </c>
       <c r="C992">
-        <v>26.794871794871788</v>
+        <v>29.794871794871799</v>
       </c>
       <c r="D992" t="s">
         <v>16</v>
@@ -21516,7 +21516,7 @@
         <v>235</v>
       </c>
       <c r="C993">
-        <v>26.794871794871788</v>
+        <v>33</v>
       </c>
       <c r="D993" t="s">
         <v>16</v>
@@ -21556,7 +21556,7 @@
         <v>238</v>
       </c>
       <c r="C995">
-        <v>26.794871794871788</v>
+        <v>32.794871794871803</v>
       </c>
       <c r="D995" t="s">
         <v>16</v>

</xml_diff>